<commit_message>
update code & county datasets to include the metro and urbanicity variables
</commit_message>
<xml_diff>
--- a/nix_shjarback_ois_mortality_preprint/data/california/ca_county_hospital.xlsx
+++ b/nix_shjarback_ois_mortality_preprint/data/california/ca_county_hospital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnshjarback/Desktop/TX AG Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE358C5-35BD-6E4A-91B9-04A61F577540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE8B4EA-E1D2-B946-AB2B-3CF75BE4C786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="820" windowWidth="27920" windowHeight="15720" xr2:uid="{515875D6-4E44-F042-87C8-51D9BA76D418}"/>
+    <workbookView xWindow="780" yWindow="820" windowWidth="15740" windowHeight="15720" xr2:uid="{515875D6-4E44-F042-87C8-51D9BA76D418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>county_name</t>
   </si>
@@ -217,6 +217,15 @@
   </si>
   <si>
     <t>total_level2</t>
+  </si>
+  <si>
+    <t>pop_2010</t>
+  </si>
+  <si>
+    <t>rucc_2013</t>
+  </si>
+  <si>
+    <t>metro_non</t>
   </si>
 </sst>
 </file>
@@ -226,7 +235,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -580,18 +589,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71232530-B47F-F64E-A94D-C677AEF49276}">
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,8 +619,17 @@
       <c r="F1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -630,8 +648,17 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>1510271</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -650,8 +677,17 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>1175</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -670,8 +706,17 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>38091</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -690,8 +735,17 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>220000</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -710,8 +764,17 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>45578</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -730,8 +793,17 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>21419</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -750,8 +822,17 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>1049025</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -770,8 +851,17 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>28610</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -790,8 +880,17 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>181058</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -810,8 +909,17 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>930450</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -830,8 +938,17 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>28122</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -850,8 +967,17 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>134623</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -870,8 +996,17 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>174528</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -890,8 +1025,17 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>18546</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -910,8 +1054,17 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>839631</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -930,8 +1083,17 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>152982</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
@@ -950,8 +1112,17 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>64665</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -970,8 +1141,17 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>34895</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
@@ -990,8 +1170,17 @@
       <c r="F20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>9818605</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -1010,8 +1199,17 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>150865</v>
+      </c>
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -1030,8 +1228,17 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>252409</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
@@ -1050,8 +1257,17 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>18251</v>
+      </c>
+      <c r="H23">
+        <v>8</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1070,8 +1286,17 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>87841</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
@@ -1090,8 +1315,17 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>255793</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
@@ -1110,8 +1344,17 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>9686</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1130,8 +1373,17 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>14202</v>
+      </c>
+      <c r="H27">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
@@ -1150,8 +1402,17 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>415057</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
@@ -1170,8 +1431,17 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>136484</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
@@ -1190,8 +1460,17 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>98764</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -1210,8 +1489,17 @@
       <c r="F31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>3010232</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -1230,8 +1518,17 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>348432</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>35</v>
       </c>
@@ -1250,8 +1547,17 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>20007</v>
+      </c>
+      <c r="H33">
+        <v>7</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>36</v>
       </c>
@@ -1270,8 +1576,17 @@
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>2189641</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
@@ -1290,8 +1605,17 @@
       <c r="F35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>1418788</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1310,8 +1634,17 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>55269</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
@@ -1330,8 +1663,17 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>2035210</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
@@ -1350,8 +1692,17 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>3095313</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>41</v>
       </c>
@@ -1370,8 +1721,17 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>805235</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -1390,8 +1750,17 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>685306</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>43</v>
       </c>
@@ -1410,8 +1779,17 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>269637</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1430,8 +1808,17 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>718451</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>45</v>
       </c>
@@ -1450,8 +1837,17 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>423895</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -1470,8 +1866,17 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>1781642</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>47</v>
       </c>
@@ -1490,8 +1895,17 @@
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>262382</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>48</v>
       </c>
@@ -1510,8 +1924,17 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>177223</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>49</v>
       </c>
@@ -1530,8 +1953,17 @@
       <c r="F47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>3240</v>
+      </c>
+      <c r="H47">
+        <v>8</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>50</v>
       </c>
@@ -1550,8 +1982,17 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>44900</v>
+      </c>
+      <c r="H48">
+        <v>6</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>51</v>
       </c>
@@ -1570,8 +2011,17 @@
       <c r="F49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>413344</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>52</v>
       </c>
@@ -1590,8 +2040,17 @@
       <c r="F50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>483878</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
@@ -1610,8 +2069,17 @@
       <c r="F51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>514453</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
@@ -1630,8 +2098,17 @@
       <c r="F52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>94737</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>55</v>
       </c>
@@ -1650,8 +2127,17 @@
       <c r="F53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <v>63463</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>56</v>
       </c>
@@ -1670,8 +2156,17 @@
       <c r="F54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <v>13786</v>
+      </c>
+      <c r="H54">
+        <v>8</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
@@ -1690,8 +2185,17 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <v>442179</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
@@ -1710,8 +2214,17 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <v>55365</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
@@ -1730,8 +2243,17 @@
       <c r="F57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <v>823318</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>60</v>
       </c>
@@ -1750,8 +2272,17 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>200849</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
@@ -1770,8 +2301,17 @@
       <c r="F59">
         <v>0</v>
       </c>
-    </row>
-    <row r="1048576" spans="6:6">
+      <c r="G59">
+        <v>72155</v>
+      </c>
+      <c r="H59">
+        <v>3</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F1048576">
         <f>SUM(F2:F1048575)</f>
         <v>37</v>

</xml_diff>